<commit_message>
Feat: Adiciona validador visual de inputs (Sanity Check)
</commit_message>
<xml_diff>
--- a/tests/output_mock/2025-11-30 - [StoneLab] Analytics presenca.xlsx
+++ b/tests/output_mock/2025-11-30 - [StoneLab] Analytics presenca.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1176" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1168" uniqueCount="214">
   <si>
     <t>nome_entrada</t>
   </si>
@@ -616,6 +616,9 @@
   </si>
   <si>
     <t>(1) Amarelo (&gt; 15 dias)</t>
+  </si>
+  <si>
+    <t>(4) Risco Inicial (10-15 dias)</t>
   </si>
   <si>
     <t>hassan touati</t>
@@ -1295,7 +1298,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1306,7 +1309,7 @@
     <col min="3" max="3" width="18.7109375" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
-    <col min="6" max="6" width="26.7109375" customWidth="1"/>
+    <col min="6" max="6" width="32.7109375" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1490,13 +1493,13 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>82</v>
+        <v>108</v>
       </c>
       <c r="B9" t="s">
         <v>179</v>
       </c>
       <c r="C9" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D9" s="2">
         <v>45950</v>
@@ -1513,13 +1516,13 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
       <c r="B10" t="s">
         <v>179</v>
       </c>
       <c r="C10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D10" s="2">
         <v>45950</v>
@@ -1536,19 +1539,19 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="B11" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C11" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D11" s="2">
-        <v>45962</v>
+        <v>45971</v>
       </c>
       <c r="E11">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F11" t="s">
         <v>196</v>
@@ -1559,19 +1562,19 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>89</v>
+        <v>106</v>
       </c>
       <c r="B12" t="s">
         <v>179</v>
       </c>
       <c r="C12" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="D12" s="2">
-        <v>45969</v>
+        <v>45971</v>
       </c>
       <c r="E12">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F12" t="s">
         <v>196</v>
@@ -1582,22 +1585,22 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="B13" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D13" s="2">
-        <v>45969</v>
+        <v>45978</v>
       </c>
       <c r="E13">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F13" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G13" s="3">
         <v>45991</v>
@@ -1605,22 +1608,22 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="B14" t="s">
         <v>180</v>
       </c>
       <c r="C14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D14" s="2">
-        <v>45976</v>
+        <v>45978</v>
       </c>
       <c r="E14">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F14" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G14" s="3">
         <v>45991</v>
@@ -1628,75 +1631,29 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="B15" t="s">
         <v>182</v>
       </c>
       <c r="C15" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D15" s="2">
-        <v>45976</v>
+        <v>45978</v>
       </c>
       <c r="E15">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F15" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G15" s="3">
         <v>45991</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
-      <c r="A16" t="s">
-        <v>85</v>
-      </c>
-      <c r="B16" t="s">
-        <v>180</v>
-      </c>
-      <c r="C16" t="s">
-        <v>124</v>
-      </c>
-      <c r="D16" s="2">
-        <v>45976</v>
-      </c>
-      <c r="E16">
-        <v>15</v>
-      </c>
-      <c r="F16" t="s">
-        <v>196</v>
-      </c>
-      <c r="G16" s="3">
-        <v>45991</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" t="s">
-        <v>116</v>
-      </c>
-      <c r="B17" t="s">
-        <v>182</v>
-      </c>
-      <c r="C17" t="s">
-        <v>123</v>
-      </c>
-      <c r="D17" s="2">
-        <v>45976</v>
-      </c>
-      <c r="E17">
-        <v>15</v>
-      </c>
-      <c r="F17" t="s">
-        <v>196</v>
-      </c>
-      <c r="G17" s="3">
-        <v>45991</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="F2:F18">
+  <conditionalFormatting sqref="F2:F16">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Vermelho">
       <formula>NOT(ISERROR(SEARCH("Vermelho",F2)))</formula>
     </cfRule>
@@ -1737,7 +1694,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B2" s="2">
         <v>45775</v>
@@ -1748,7 +1705,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B3" s="2">
         <v>45775</v>
@@ -1759,7 +1716,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B4" s="2">
         <v>45775</v>
@@ -1770,7 +1727,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B5" s="2">
         <v>45775</v>
@@ -1781,7 +1738,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B6" s="2">
         <v>45775</v>
@@ -1792,7 +1749,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B7" s="2">
         <v>45803</v>
@@ -1803,7 +1760,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B8" s="2">
         <v>45803</v>
@@ -1814,7 +1771,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B9" s="2">
         <v>45803</v>
@@ -1825,7 +1782,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B10" s="2">
         <v>45803</v>
@@ -1836,7 +1793,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B11" s="2">
         <v>45803</v>
@@ -1847,7 +1804,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B12" s="2">
         <v>45838</v>
@@ -1858,7 +1815,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B13" s="2">
         <v>45866</v>
@@ -1869,7 +1826,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B14" s="2">
         <v>45866</v>
@@ -1880,7 +1837,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B15" s="2">
         <v>45894</v>
@@ -1891,7 +1848,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B16" s="2">
         <v>45894</v>
@@ -1902,7 +1859,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B17" s="2">
         <v>45894</v>

</xml_diff>